<commit_message>
moved convert logic from function to class
</commit_message>
<xml_diff>
--- a/dev/fleet.xlsx
+++ b/dev/fleet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Apps\django-from-excel\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D8B8144-2876-4FC8-908A-75BAA0267BFD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8E4440-4828-4E91-B3AC-871A62554856}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fleet" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>VIN</t>
   </si>
@@ -440,7 +440,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -602,9 +602,6 @@
       <c r="G5">
         <v>4.5999999999999996</v>
       </c>
-      <c r="H5" t="s">
-        <v>20</v>
-      </c>
       <c r="I5">
         <v>26.348290348203399</v>
       </c>

</xml_diff>